<commit_message>
Remove dead code and add extra test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/timing_check.xlsx
+++ b/tests/integration_test_files/timing_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6556F773-68BB-C243-95E8-F9342AA85F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDACB45A-E816-E044-BCF7-825771ECD2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26920" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="7" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="49420" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="7" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="827">
   <si>
     <t>Screening</t>
   </si>
@@ -2554,6 +2554,15 @@
   </si>
   <si>
     <t>DOSExx</t>
+  </si>
+  <si>
+    <t>BP_STANDxxx</t>
+  </si>
+  <si>
+    <t>EXTRA</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
@@ -2795,13 +2804,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3781,10 +3790,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A98DD9-8159-D74D-B42C-CCC2F4D10811}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3792,10 +3801,10 @@
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="53.6640625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="16" style="1" customWidth="1"/>
+    <col min="4" max="8" width="16" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
@@ -3815,10 +3824,13 @@
         <v>723</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>84</v>
       </c>
@@ -3830,7 +3842,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>86</v>
       </c>
@@ -3850,10 +3862,13 @@
         <v>727</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="17" t="s">
@@ -3871,8 +3886,11 @@
       <c r="G4" s="2" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
@@ -3888,31 +3906,34 @@
         <v>721</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -3923,7 +3944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>742</v>
@@ -3935,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
         <v>729</v>
@@ -3947,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
         <v>743</v>
@@ -3959,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>730</v>
@@ -3967,22 +3988,22 @@
       <c r="C13" s="16" t="s">
         <v>722</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
@@ -4103,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B8B105-0AE3-CA42-845E-0FC79C427790}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4735,7 +4756,7 @@
         <v>550</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>721</v>
+        <v>824</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>723</v>
@@ -7963,120 +7984,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>684</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>719</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8168,16 +8189,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11800,15 +11821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
@@ -11817,6 +11829,15 @@
     <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12021,14 +12042,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12041,6 +12054,14 @@
     <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>